<commit_message>
Update Eletrical template files
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_Cable_Condiut_MatchTable_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_Cable_Condiut_MatchTable_19DX101.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203C8971-A6CB-428C-A2F8-0FB2643B557D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="15792" yWindow="252" windowWidth="13308" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15795" yWindow="255" windowWidth="13305" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="YJY(YJV)" sheetId="1" r:id="rId1"/>
     <sheet name="BYJ(BV)" sheetId="3" r:id="rId2"/>
+    <sheet name="KYJY(KYJV)" sheetId="4" r:id="rId3"/>
+    <sheet name="RYJ" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
   <si>
     <t>DIN(SC)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,11 +79,30 @@
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>控制线导体截面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制线芯数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Wires</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,10 +139,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,19 +432,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="6" width="12.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -435,7 +464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -455,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -475,7 +504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -495,7 +524,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -515,7 +544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -535,7 +564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -555,7 +584,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -575,7 +604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -595,7 +624,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -609,7 +638,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -623,7 +652,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -637,7 +666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -651,7 +680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -665,7 +694,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -679,7 +708,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -693,7 +722,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -707,7 +736,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -721,7 +750,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,7 +764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -749,7 +778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -763,7 +792,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -777,7 +806,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -791,7 +820,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -805,7 +834,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -819,7 +848,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -833,7 +862,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -847,7 +876,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -861,7 +890,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -875,7 +904,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -897,19 +926,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="6" width="12.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -929,7 +958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -949,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>2.5</v>
       </c>
@@ -966,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2.5</v>
       </c>
@@ -983,7 +1012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -1000,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1017,7 +1046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -1034,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1051,7 +1080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>10</v>
       </c>
@@ -1068,7 +1097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>10</v>
       </c>
@@ -1085,7 +1114,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>16</v>
       </c>
@@ -1102,7 +1131,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>16</v>
       </c>
@@ -1119,7 +1148,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>25</v>
       </c>
@@ -1136,7 +1165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>25</v>
       </c>
@@ -1150,7 +1179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>35</v>
       </c>
@@ -1167,7 +1196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>35</v>
       </c>
@@ -1178,7 +1207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>50</v>
       </c>
@@ -1195,7 +1224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>50</v>
       </c>
@@ -1206,7 +1235,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>70</v>
       </c>
@@ -1217,7 +1246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>70</v>
       </c>
@@ -1228,7 +1257,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>95</v>
       </c>
@@ -1239,7 +1268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>95</v>
       </c>
@@ -1250,7 +1279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>120</v>
       </c>
@@ -1261,7 +1290,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>120</v>
       </c>
@@ -1277,4 +1306,2006 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>25</v>
+      </c>
+      <c r="E10" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3">
+        <v>32</v>
+      </c>
+      <c r="E20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>40</v>
+      </c>
+      <c r="D21" s="3">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3">
+        <v>40</v>
+      </c>
+      <c r="E22" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3">
+        <v>40</v>
+      </c>
+      <c r="E24" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3">
+        <v>40</v>
+      </c>
+      <c r="D25" s="3">
+        <v>40</v>
+      </c>
+      <c r="E25" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3">
+        <v>40</v>
+      </c>
+      <c r="D26" s="3">
+        <v>40</v>
+      </c>
+      <c r="E26" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3">
+        <v>40</v>
+      </c>
+      <c r="D27" s="3">
+        <v>40</v>
+      </c>
+      <c r="E27" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3">
+        <v>40</v>
+      </c>
+      <c r="D28" s="3">
+        <v>40</v>
+      </c>
+      <c r="E28" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3">
+        <v>50</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3">
+        <v>50</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>20</v>
+      </c>
+      <c r="D32" s="3">
+        <v>20</v>
+      </c>
+      <c r="E32" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>25</v>
+      </c>
+      <c r="D33" s="3">
+        <v>25</v>
+      </c>
+      <c r="E33" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B34" s="3">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3">
+        <v>25</v>
+      </c>
+      <c r="D34" s="3">
+        <v>25</v>
+      </c>
+      <c r="E34" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3">
+        <v>25</v>
+      </c>
+      <c r="E35" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B36" s="3">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>32</v>
+      </c>
+      <c r="E36" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B37" s="3">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3">
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>32</v>
+      </c>
+      <c r="E37" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B38" s="3">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3">
+        <v>32</v>
+      </c>
+      <c r="D38" s="3">
+        <v>32</v>
+      </c>
+      <c r="E38" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B39" s="3">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3">
+        <v>40</v>
+      </c>
+      <c r="D39" s="3">
+        <v>40</v>
+      </c>
+      <c r="E39" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B40" s="3">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3">
+        <v>40</v>
+      </c>
+      <c r="D40" s="3">
+        <v>40</v>
+      </c>
+      <c r="E40" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B41" s="3">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3">
+        <v>40</v>
+      </c>
+      <c r="D41" s="3">
+        <v>40</v>
+      </c>
+      <c r="E41" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B42" s="3">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3">
+        <v>40</v>
+      </c>
+      <c r="E42" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B43" s="3">
+        <v>13</v>
+      </c>
+      <c r="C43" s="3">
+        <v>40</v>
+      </c>
+      <c r="D43" s="3">
+        <v>40</v>
+      </c>
+      <c r="E43" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B44" s="3">
+        <v>14</v>
+      </c>
+      <c r="C44" s="3">
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>40</v>
+      </c>
+      <c r="E44" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>15</v>
+      </c>
+      <c r="C45" s="3">
+        <v>50</v>
+      </c>
+      <c r="D45" s="3">
+        <v>50</v>
+      </c>
+      <c r="E45" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B46" s="3">
+        <v>16</v>
+      </c>
+      <c r="C46" s="3">
+        <v>50</v>
+      </c>
+      <c r="D46" s="3">
+        <v>50</v>
+      </c>
+      <c r="E46" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B47" s="3">
+        <v>17</v>
+      </c>
+      <c r="C47" s="3">
+        <v>50</v>
+      </c>
+      <c r="D47" s="3">
+        <v>50</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B48" s="3">
+        <v>18</v>
+      </c>
+      <c r="C48" s="3">
+        <v>50</v>
+      </c>
+      <c r="D48" s="3">
+        <v>50</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B49" s="3">
+        <v>19</v>
+      </c>
+      <c r="C49" s="3">
+        <v>50</v>
+      </c>
+      <c r="D49" s="3">
+        <v>50</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B50" s="3">
+        <v>20</v>
+      </c>
+      <c r="C50" s="3">
+        <v>50</v>
+      </c>
+      <c r="D50" s="3">
+        <v>50</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B51" s="3">
+        <v>21</v>
+      </c>
+      <c r="C51" s="3">
+        <v>50</v>
+      </c>
+      <c r="D51" s="3">
+        <v>50</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B52" s="3">
+        <v>22</v>
+      </c>
+      <c r="C52" s="3">
+        <v>50</v>
+      </c>
+      <c r="D52" s="3">
+        <v>50</v>
+      </c>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B53" s="3">
+        <v>23</v>
+      </c>
+      <c r="C53" s="3">
+        <v>50</v>
+      </c>
+      <c r="D53" s="3">
+        <v>50</v>
+      </c>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B54" s="3">
+        <v>24</v>
+      </c>
+      <c r="C54" s="3">
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>50</v>
+      </c>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B55" s="3">
+        <v>25</v>
+      </c>
+      <c r="C55" s="3">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3">
+        <v>65</v>
+      </c>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B56" s="3">
+        <v>26</v>
+      </c>
+      <c r="C56" s="3">
+        <v>65</v>
+      </c>
+      <c r="D56" s="3">
+        <v>65</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B57" s="3">
+        <v>27</v>
+      </c>
+      <c r="C57" s="3">
+        <v>65</v>
+      </c>
+      <c r="D57" s="3">
+        <v>65</v>
+      </c>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B58" s="3">
+        <v>28</v>
+      </c>
+      <c r="C58" s="3">
+        <v>65</v>
+      </c>
+      <c r="D58" s="3">
+        <v>65</v>
+      </c>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B59" s="3">
+        <v>29</v>
+      </c>
+      <c r="C59" s="3">
+        <v>65</v>
+      </c>
+      <c r="D59" s="3">
+        <v>65</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B60" s="3">
+        <v>30</v>
+      </c>
+      <c r="C60" s="3">
+        <v>65</v>
+      </c>
+      <c r="D60" s="3">
+        <v>65</v>
+      </c>
+      <c r="E60" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>25</v>
+      </c>
+      <c r="E10" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3">
+        <v>32</v>
+      </c>
+      <c r="E20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>40</v>
+      </c>
+      <c r="D21" s="3">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3">
+        <v>40</v>
+      </c>
+      <c r="E22" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3">
+        <v>40</v>
+      </c>
+      <c r="E24" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3">
+        <v>40</v>
+      </c>
+      <c r="D25" s="3">
+        <v>40</v>
+      </c>
+      <c r="E25" s="3">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3">
+        <v>40</v>
+      </c>
+      <c r="D26" s="3">
+        <v>40</v>
+      </c>
+      <c r="E26" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3">
+        <v>40</v>
+      </c>
+      <c r="D27" s="3">
+        <v>40</v>
+      </c>
+      <c r="E27" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3">
+        <v>40</v>
+      </c>
+      <c r="D28" s="3">
+        <v>40</v>
+      </c>
+      <c r="E28" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>20</v>
+      </c>
+      <c r="D32" s="3">
+        <v>20</v>
+      </c>
+      <c r="E32" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>25</v>
+      </c>
+      <c r="D33" s="3">
+        <v>25</v>
+      </c>
+      <c r="E33" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B34" s="3">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3">
+        <v>25</v>
+      </c>
+      <c r="D34" s="3">
+        <v>25</v>
+      </c>
+      <c r="E34" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3">
+        <v>25</v>
+      </c>
+      <c r="E35" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B36" s="3">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>32</v>
+      </c>
+      <c r="E36" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B37" s="3">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3">
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>32</v>
+      </c>
+      <c r="E37" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B38" s="3">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3">
+        <v>32</v>
+      </c>
+      <c r="D38" s="3">
+        <v>32</v>
+      </c>
+      <c r="E38" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B39" s="3">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3">
+        <v>40</v>
+      </c>
+      <c r="D39" s="3">
+        <v>40</v>
+      </c>
+      <c r="E39" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B40" s="3">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3">
+        <v>40</v>
+      </c>
+      <c r="D40" s="3">
+        <v>40</v>
+      </c>
+      <c r="E40" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B41" s="3">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3">
+        <v>40</v>
+      </c>
+      <c r="D41" s="3">
+        <v>40</v>
+      </c>
+      <c r="E41" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B42" s="3">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3">
+        <v>40</v>
+      </c>
+      <c r="E42" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B43" s="3">
+        <v>13</v>
+      </c>
+      <c r="C43" s="3">
+        <v>40</v>
+      </c>
+      <c r="D43" s="3">
+        <v>40</v>
+      </c>
+      <c r="E43" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B44" s="3">
+        <v>14</v>
+      </c>
+      <c r="C44" s="3">
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>40</v>
+      </c>
+      <c r="E44" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>15</v>
+      </c>
+      <c r="C45" s="3">
+        <v>50</v>
+      </c>
+      <c r="D45" s="3">
+        <v>50</v>
+      </c>
+      <c r="E45" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B46" s="3">
+        <v>16</v>
+      </c>
+      <c r="C46" s="3">
+        <v>50</v>
+      </c>
+      <c r="D46" s="3">
+        <v>50</v>
+      </c>
+      <c r="E46" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B47" s="3">
+        <v>17</v>
+      </c>
+      <c r="C47" s="3">
+        <v>50</v>
+      </c>
+      <c r="D47" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B48" s="3">
+        <v>18</v>
+      </c>
+      <c r="C48" s="3">
+        <v>50</v>
+      </c>
+      <c r="D48" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B49" s="3">
+        <v>19</v>
+      </c>
+      <c r="C49" s="3">
+        <v>50</v>
+      </c>
+      <c r="D49" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B50" s="3">
+        <v>20</v>
+      </c>
+      <c r="C50" s="3">
+        <v>50</v>
+      </c>
+      <c r="D50" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B51" s="3">
+        <v>21</v>
+      </c>
+      <c r="C51" s="3">
+        <v>50</v>
+      </c>
+      <c r="D51" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B52" s="3">
+        <v>22</v>
+      </c>
+      <c r="C52" s="3">
+        <v>50</v>
+      </c>
+      <c r="D52" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B53" s="3">
+        <v>23</v>
+      </c>
+      <c r="C53" s="3">
+        <v>50</v>
+      </c>
+      <c r="D53" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B54" s="3">
+        <v>24</v>
+      </c>
+      <c r="C54" s="3">
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B55" s="3">
+        <v>25</v>
+      </c>
+      <c r="C55" s="3">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B56" s="3">
+        <v>26</v>
+      </c>
+      <c r="C56" s="3">
+        <v>65</v>
+      </c>
+      <c r="D56" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B57" s="3">
+        <v>27</v>
+      </c>
+      <c r="C57" s="3">
+        <v>65</v>
+      </c>
+      <c r="D57" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B58" s="3">
+        <v>28</v>
+      </c>
+      <c r="C58" s="3">
+        <v>65</v>
+      </c>
+      <c r="D58" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B59" s="3">
+        <v>29</v>
+      </c>
+      <c r="C59" s="3">
+        <v>65</v>
+      </c>
+      <c r="D59" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B60" s="3">
+        <v>30</v>
+      </c>
+      <c r="C60" s="3">
+        <v>65</v>
+      </c>
+      <c r="D60" s="3">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>